<commit_message>
Tilpasset modell for inntak av excel.
</commit_message>
<xml_diff>
--- a/productdata.xlsx
+++ b/productdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varsh\PycharmProjects\SizingOffGridMicrogrids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D289DFF4-FA16-43A8-BEF7-35F4C08678B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1BCCC1-63C2-4BE1-8D8D-DD8236A50D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18120" yWindow="-4680" windowWidth="18240" windowHeight="28440" xr2:uid="{DB6903CB-CB73-439C-BE90-89BBD3CE7FA7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Input" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,6 +33,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>PV1</t>
+  </si>
+  <si>
+    <t>PV2</t>
+  </si>
+  <si>
+    <t>PV3</t>
+  </si>
+  <si>
+    <t>Battery1</t>
+  </si>
+  <si>
+    <t>Battery2</t>
+  </si>
+  <si>
+    <t>Battery3</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,12 +405,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713CAAAD-4950-4AF3-9D13-2034DE5C9FF9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G9:G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>300</v>
+      </c>
+      <c r="D2">
+        <v>500</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>150</v>
+      </c>
+      <c r="B3">
+        <v>250</v>
+      </c>
+      <c r="C3">
+        <v>350</v>
+      </c>
+      <c r="D3">
+        <v>7000</v>
+      </c>
+      <c r="E3">
+        <v>1500</v>
+      </c>
+      <c r="F3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>200</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4">
+        <v>400</v>
+      </c>
+      <c r="D4">
+        <v>900</v>
+      </c>
+      <c r="E4">
+        <v>2000</v>
+      </c>
+      <c r="F4">
+        <v>4000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Legger til henting fra excel + lager ny analysis fil
</commit_message>
<xml_diff>
--- a/productdata.xlsx
+++ b/productdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varsh\PycharmProjects\SizingOffGridMicrogrids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1BCCC1-63C2-4BE1-8D8D-DD8236A50D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1873F786-E604-49A6-AE94-FC4D579A7306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18120" yWindow="-4680" windowWidth="18240" windowHeight="28440" xr2:uid="{DB6903CB-CB73-439C-BE90-89BBD3CE7FA7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DB6903CB-CB73-439C-BE90-89BBD3CE7FA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>PV1</t>
   </si>
@@ -54,14 +54,49 @@
   </si>
   <si>
     <t>Battery3</t>
+  </si>
+  <si>
+    <t>Enhet</t>
+  </si>
+  <si>
+    <t>Watt</t>
+  </si>
+  <si>
+    <t>Pris</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>MaxPower</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -89,8 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,95 +441,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713CAAAD-4950-4AF3-9D13-2034DE5C9FF9}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G9:G10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
         <v>100</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>200</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>300</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>500</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1000</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
         <v>150</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>250</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>350</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>7000</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1500</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
         <v>200</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>300</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>400</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>900</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2000</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>4000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Delt opp i faner i excel, lagt inn for load men man vil knaskje ha det fra et eget dokument?.
</commit_message>
<xml_diff>
--- a/productdata.xlsx
+++ b/productdata.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varsh\PycharmProjects\SizingOffGridMicrogrids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1873F786-E604-49A6-AE94-FC4D579A7306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A308FF07-D8EE-4B2C-A6B7-2BF4284DE8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DB6903CB-CB73-439C-BE90-89BBD3CE7FA7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DB6903CB-CB73-439C-BE90-89BBD3CE7FA7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Input" sheetId="1" r:id="rId1"/>
+    <sheet name="Battery" sheetId="2" r:id="rId1"/>
+    <sheet name="PV" sheetId="3" r:id="rId2"/>
+    <sheet name="Load" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>PV1</t>
   </si>
@@ -68,9 +70,6 @@
     <t>Capacity</t>
   </si>
   <si>
-    <t>Efficiency</t>
-  </si>
-  <si>
     <t>0.9</t>
   </si>
   <si>
@@ -80,7 +79,37 @@
     <t>0.5</t>
   </si>
   <si>
-    <t>MaxPower</t>
+    <t>xfgdfg</t>
+  </si>
+  <si>
+    <t>P_max</t>
+  </si>
+  <si>
+    <t>v_oc</t>
+  </si>
+  <si>
+    <t>i_sc</t>
+  </si>
+  <si>
+    <t>alpha_sc</t>
+  </si>
+  <si>
+    <t>beta_voc</t>
+  </si>
+  <si>
+    <t>gamma_pmp</t>
+  </si>
+  <si>
+    <t>temp_ref</t>
+  </si>
+  <si>
+    <t>surface_tilt</t>
+  </si>
+  <si>
+    <t>surface_azimuth</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -440,131 +469,276 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713CAAAD-4950-4AF3-9D13-2034DE5C9FF9}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AC6BE0-FB58-4ADE-BBC4-B8CFC61971DC}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>7000</v>
+      </c>
+      <c r="C3">
+        <v>1500</v>
+      </c>
+      <c r="D3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>900</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+      <c r="D4">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F84E61-4F05-4493-8F01-DF88A633332D}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>49.84</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>50.16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>11.34</v>
+      </c>
+      <c r="C4">
+        <v>12.45</v>
+      </c>
+      <c r="D4">
+        <v>13.56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <f>0.0006*B4</f>
+        <v>6.8039999999999993E-3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:D5" si="0">0.0006*C4</f>
+        <v>7.4699999999999992E-3</v>
+      </c>
+      <c r="D5">
+        <f>0.0006*D4</f>
+        <v>8.1359999999999991E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <f xml:space="preserve"> -0.003*B3</f>
+        <v>-0.14952000000000001</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:D6" si="1" xml:space="preserve"> -0.003*C3</f>
+        <v>-0.15</v>
+      </c>
+      <c r="D6">
+        <f xml:space="preserve"> -0.003*D3</f>
+        <v>-0.15048</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>-3.8999999999999998E-3</v>
+      </c>
+      <c r="C7">
+        <v>-3.8999999999999998E-3</v>
+      </c>
+      <c r="D7">
+        <v>-3.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>6.2</v>
+      </c>
+      <c r="C9">
+        <v>6.2</v>
+      </c>
+      <c r="D9">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>-50</v>
+      </c>
+      <c r="C10">
+        <v>-50</v>
+      </c>
+      <c r="D10">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
         <v>100</v>
       </c>
-      <c r="C2">
-        <v>200</v>
-      </c>
-      <c r="D2">
-        <v>300</v>
-      </c>
-      <c r="E2">
-        <v>500</v>
-      </c>
-      <c r="F2">
-        <v>1000</v>
-      </c>
-      <c r="G2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>150</v>
-      </c>
-      <c r="C3">
-        <v>250</v>
-      </c>
-      <c r="D3">
-        <v>350</v>
-      </c>
-      <c r="E3">
-        <v>7000</v>
-      </c>
-      <c r="F3">
-        <v>1500</v>
-      </c>
-      <c r="G3">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>200</v>
-      </c>
-      <c r="C4">
-        <v>300</v>
-      </c>
-      <c r="D4">
-        <v>400</v>
-      </c>
-      <c r="E4">
-        <v>900</v>
-      </c>
-      <c r="F4">
-        <v>2000</v>
-      </c>
-      <c r="G4">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
+      <c r="C11">
+        <v>110</v>
+      </c>
+      <c r="D11">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531FD1E1-11A8-4863-90E1-7CB24B554877}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>